<commit_message>
Deploy data to app repo
</commit_message>
<xml_diff>
--- a/data/xlsx/Baernreither_Index_2023.xlsx
+++ b/data/xlsx/Baernreither_Index_2023.xlsx
@@ -1,22 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christofaichner/Documents/GitHub/baernreither-data/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2715E89D-1A5C-6542-8D98-6DC7249098A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8942E3D-D22A-AC40-9C06-A95546E18D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="MIGAEtrWxjvykv7E4pmlZvogrId1c8BxcQ5Ejh8Kqvs="/>
     </ext>
@@ -1202,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC1034"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>

</xml_diff>